<commit_message>
ia and monitor tabs
</commit_message>
<xml_diff>
--- a/sections_config.xlsx
+++ b/sections_config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/13a0fd42d83c08bf/Documents/Cursos/ILLINOIS/IE_421_High_Frequency_Trading/LinuxVM/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{17DEADED-3F36-7A45-9954-13B779C8B78F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{755D258A-656B-1949-94DD-80B61EAE2CD7}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{17DEADED-3F36-7A45-9954-13B779C8B78F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00775444-452E-3E42-A0C7-37908564D0D0}"/>
   <bookViews>
     <workbookView xWindow="1480" yWindow="1660" windowWidth="27240" windowHeight="16160" xr2:uid="{D840E18A-208A-1543-8781-3BD2E5582C66}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="134">
   <si>
     <t>Section_Title</t>
   </si>
@@ -429,6 +429,15 @@
   </si>
   <si>
     <t xml:space="preserve">custom </t>
+  </si>
+  <si>
+    <t>Threshold_Min</t>
+  </si>
+  <si>
+    <t>Threshold_Max</t>
+  </si>
+  <si>
+    <t>Unit</t>
   </si>
 </sst>
 </file>
@@ -821,10 +830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F98F07-8A77-3547-A6A2-1E1EBA77126D}">
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -832,10 +841,10 @@
     <col min="1" max="1" width="27.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="144.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="144.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -848,8 +857,17 @@
       <c r="D1" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>50</v>
       </c>
@@ -863,7 +881,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -877,7 +895,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -891,7 +909,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -905,7 +923,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -919,7 +937,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -933,7 +951,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -947,7 +965,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -961,7 +979,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -975,7 +993,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
@@ -989,7 +1007,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -1003,7 +1021,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -1017,7 +1035,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -1031,7 +1049,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -1045,7 +1063,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Performance tab + Ai
</commit_message>
<xml_diff>
--- a/sections_config.xlsx
+++ b/sections_config.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/13a0fd42d83c08bf/Documents/Cursos/ILLINOIS/IE_421_High_Frequency_Trading/LinuxVM/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{17DEADED-3F36-7A45-9954-13B779C8B78F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00775444-452E-3E42-A0C7-37908564D0D0}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="8_{17DEADED-3F36-7A45-9954-13B779C8B78F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2BC6806-065A-0848-B249-98B965329BD7}"/>
   <bookViews>
     <workbookView xWindow="1480" yWindow="1660" windowWidth="27240" windowHeight="16160" xr2:uid="{D840E18A-208A-1543-8781-3BD2E5582C66}"/>
   </bookViews>
   <sheets>
     <sheet name="Sections" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sections!$A$1:$H$57</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="141">
   <si>
     <t>Section_Title</t>
   </si>
@@ -438,6 +441,27 @@
   </si>
   <si>
     <t>Unit</t>
+  </si>
+  <si>
+    <t>HFT_Profile</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>LowLatency</t>
+  </si>
+  <si>
+    <t>Network</t>
+  </si>
+  <si>
+    <t>Memory</t>
+  </si>
+  <si>
+    <t>Storage</t>
+  </si>
+  <si>
+    <t>Custom</t>
   </si>
 </sst>
 </file>
@@ -830,10 +854,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F98F07-8A77-3547-A6A2-1E1EBA77126D}">
-  <dimension ref="A1:G57"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -844,7 +869,7 @@
     <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -866,8 +891,11 @@
       <c r="G1" s="2" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>50</v>
       </c>
@@ -880,8 +908,11 @@
       <c r="D2" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -894,8 +925,11 @@
       <c r="D3" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -908,8 +942,11 @@
       <c r="D4" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -922,8 +959,11 @@
       <c r="D5" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -936,8 +976,11 @@
       <c r="D6" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -950,8 +993,11 @@
       <c r="D7" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -964,8 +1010,11 @@
       <c r="D8" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -978,8 +1027,11 @@
       <c r="D9" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -992,8 +1044,11 @@
       <c r="D10" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
@@ -1006,8 +1061,11 @@
       <c r="D11" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -1020,8 +1078,11 @@
       <c r="D12" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -1034,8 +1095,11 @@
       <c r="D13" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H13" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -1048,8 +1112,11 @@
       <c r="D14" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H14" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -1062,8 +1129,11 @@
       <c r="D15" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H15" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -1076,8 +1146,11 @@
       <c r="D16" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
@@ -1090,8 +1163,11 @@
       <c r="D17" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H17" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>56</v>
       </c>
@@ -1104,8 +1180,11 @@
       <c r="D18" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H18" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>56</v>
       </c>
@@ -1118,8 +1197,11 @@
       <c r="D19" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H19" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>61</v>
       </c>
@@ -1132,8 +1214,11 @@
       <c r="D20" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H20" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>63</v>
       </c>
@@ -1146,8 +1231,11 @@
       <c r="D21" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H21" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>66</v>
       </c>
@@ -1160,8 +1248,11 @@
       <c r="D22" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H22" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>69</v>
       </c>
@@ -1174,8 +1265,11 @@
       <c r="D23" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H23" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>69</v>
       </c>
@@ -1188,8 +1282,11 @@
       <c r="D24" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H24" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>74</v>
       </c>
@@ -1202,8 +1299,11 @@
       <c r="D25" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H25" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>77</v>
       </c>
@@ -1216,8 +1316,11 @@
       <c r="D26" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H26" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>77</v>
       </c>
@@ -1230,8 +1333,11 @@
       <c r="D27" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H27" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>19</v>
       </c>
@@ -1244,8 +1350,11 @@
       <c r="D28" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H28" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>19</v>
       </c>
@@ -1258,8 +1367,11 @@
       <c r="D29" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H29" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>19</v>
       </c>
@@ -1272,8 +1384,11 @@
       <c r="D30" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H30" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>19</v>
       </c>
@@ -1286,8 +1401,11 @@
       <c r="D31" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H31" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>19</v>
       </c>
@@ -1300,8 +1418,11 @@
       <c r="D32" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H32" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>19</v>
       </c>
@@ -1314,8 +1435,11 @@
       <c r="D33" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H33" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>19</v>
       </c>
@@ -1328,8 +1452,11 @@
       <c r="D34" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H34" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>19</v>
       </c>
@@ -1342,8 +1469,17 @@
       <c r="D35" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E35">
+        <v>100</v>
+      </c>
+      <c r="F35">
+        <v>120</v>
+      </c>
+      <c r="H35" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>19</v>
       </c>
@@ -1356,8 +1492,17 @@
       <c r="D36" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E36">
+        <v>4000000</v>
+      </c>
+      <c r="F36">
+        <v>6000000</v>
+      </c>
+      <c r="H36" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>19</v>
       </c>
@@ -1370,8 +1515,17 @@
       <c r="D37" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37">
+        <v>4000000</v>
+      </c>
+      <c r="F37">
+        <v>6000000</v>
+      </c>
+      <c r="H37" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
@@ -1384,8 +1538,14 @@
       <c r="D38" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F38">
+        <v>5</v>
+      </c>
+      <c r="H38" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
@@ -1398,8 +1558,11 @@
       <c r="D39" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H39" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
@@ -1412,8 +1575,11 @@
       <c r="D40" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H40" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>19</v>
       </c>
@@ -1426,8 +1592,11 @@
       <c r="D41" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H41" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>19</v>
       </c>
@@ -1440,8 +1609,11 @@
       <c r="D42" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H42" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>19</v>
       </c>
@@ -1454,8 +1626,11 @@
       <c r="D43" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H43" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>19</v>
       </c>
@@ -1468,8 +1643,11 @@
       <c r="D44" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H44" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>19</v>
       </c>
@@ -1482,8 +1660,11 @@
       <c r="D45" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H45" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>19</v>
       </c>
@@ -1496,8 +1677,11 @@
       <c r="D46" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H46" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>19</v>
       </c>
@@ -1510,8 +1694,11 @@
       <c r="D47" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H47" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>19</v>
       </c>
@@ -1524,8 +1711,11 @@
       <c r="D48" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H48" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>19</v>
       </c>
@@ -1538,8 +1728,11 @@
       <c r="D49" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H49" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>27</v>
       </c>
@@ -1552,8 +1745,11 @@
       <c r="D50" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H50" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>27</v>
       </c>
@@ -1566,8 +1762,11 @@
       <c r="D51" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H51" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>114</v>
       </c>
@@ -1580,8 +1779,11 @@
       <c r="D52" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H52" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>114</v>
       </c>
@@ -1594,8 +1796,11 @@
       <c r="D53" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H53" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>114</v>
       </c>
@@ -1608,8 +1813,11 @@
       <c r="D54" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H54" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>114</v>
       </c>
@@ -1622,8 +1830,11 @@
       <c r="D55" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H55" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>114</v>
       </c>
@@ -1636,8 +1847,11 @@
       <c r="D56" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H56" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>125</v>
       </c>
@@ -1647,8 +1861,18 @@
       <c r="D57" t="s">
         <v>53</v>
       </c>
+      <c r="H57" t="s">
+        <v>140</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H57" xr:uid="{F7F98F07-8A77-3547-A6A2-1E1EBA77126D}">
+    <filterColumn colId="7">
+      <filters>
+        <filter val="Storage"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>